<commit_message>
Saturday 2/27 powerpoint, pgadmin, excel file
</commit_message>
<xml_diff>
--- a/data/app_data_excelbook.xlsx
+++ b/data/app_data_excelbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drumt\Documents\NSS_Data_Analytics\projects\app-trader-elegant-mangos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA70537-B107-48E6-821F-C52A368EA482}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64DB843-609E-48A6-BB93-073B88A79BF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C84F5E33-8A2D-49B6-ACA6-7A9717A49887}"/>
   </bookViews>
@@ -33,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="34">
   <si>
     <t>Clash of Clans</t>
   </si>
@@ -120,25 +142,22 @@
     <t>Hill Climb Racing</t>
   </si>
   <si>
-    <t>App</t>
-  </si>
-  <si>
-    <t>apple_rating</t>
-  </si>
-  <si>
-    <t>apple review count</t>
-  </si>
-  <si>
-    <t>genre</t>
-  </si>
-  <si>
-    <t>google rating</t>
-  </si>
-  <si>
-    <t>google review count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genre </t>
+    <t>game</t>
+  </si>
+  <si>
+    <t>PAC-MAN</t>
+  </si>
+  <si>
+    <t>The Sims™ FreePlay</t>
+  </si>
+  <si>
+    <t>Sonic Dash</t>
+  </si>
+  <si>
+    <t>APPLE REVIEWS</t>
+  </si>
+  <si>
+    <t>GOOGLE REVIEWS</t>
   </si>
 </sst>
 </file>
@@ -154,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +189,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,10 +240,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,19 +560,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1F18FB-012B-490B-BA80-0434436AA8E9}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.81640625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
     <col min="3" max="3" width="22.6328125" customWidth="1"/>
     <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="44.54296875" customWidth="1"/>
     <col min="7" max="7" width="14.81640625" customWidth="1"/>
     <col min="8" max="8" width="13.08984375" customWidth="1"/>
@@ -865,262 +892,270 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="E14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>4.5</v>
+      </c>
+      <c r="C15">
+        <v>2130805</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G15">
+        <v>44893888</v>
+      </c>
+      <c r="H15" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="6" t="s">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>4.5</v>
+      </c>
+      <c r="C16">
+        <v>1724546</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>4.5</v>
+      </c>
+      <c r="G16">
+        <v>27725352</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>4.5</v>
+      </c>
+      <c r="C17">
+        <v>961794</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G17">
+        <v>23136735</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>4.5</v>
+      </c>
+      <c r="C18">
+        <v>706110</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G18">
+        <v>22430188</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>4.5</v>
+      </c>
+      <c r="C19">
+        <v>698516</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>4.5</v>
+      </c>
+      <c r="G19">
+        <v>14892469</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>4.5</v>
+      </c>
+      <c r="C20">
+        <v>679055</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G20">
+        <v>10981850</v>
+      </c>
+      <c r="H20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>4.5</v>
+      </c>
+      <c r="C21">
+        <v>612532</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>4.3</v>
+      </c>
+      <c r="G21">
+        <v>10486018</v>
+      </c>
+      <c r="H21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>508808</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G22">
+        <v>10424925</v>
+      </c>
+      <c r="H22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="B23">
+        <v>4.5</v>
+      </c>
+      <c r="C23">
+        <v>446880</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23">
+        <v>4.5</v>
+      </c>
+      <c r="G23">
+        <v>9883367</v>
+      </c>
+      <c r="H23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="C15" s="6">
-        <v>2130805</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="6">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="F15" s="6">
-        <v>44893888</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="C16" s="6">
-        <v>706110</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="F16" s="6">
-        <v>27725352</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="C17" s="6">
-        <v>266921</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="6">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="F17" s="6">
-        <v>23136735</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="C18" s="6">
-        <v>961794</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="B24">
+        <v>4.5</v>
+      </c>
+      <c r="C24">
+        <v>418033</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F18" s="6">
-        <v>22430188</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="C19" s="6">
-        <v>123859</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="F19" s="6">
-        <v>14892469</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="C20" s="6">
-        <v>99206</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="6">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="F20" s="6">
-        <v>10981850</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="C21" s="6">
-        <v>3783</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="6">
-        <v>4.3</v>
-      </c>
-      <c r="F21" s="6">
-        <v>10486018</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="6">
-        <v>3</v>
-      </c>
-      <c r="C22" s="6">
-        <v>257627</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="6">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F22" s="6">
-        <v>10424925</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="C23" s="6">
-        <v>54549</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="F23" s="6">
-        <v>9883367</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="6">
-        <v>4.5</v>
-      </c>
-      <c r="C24" s="6">
-        <v>108183</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="6">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F24" s="6">
+      <c r="G24">
         <v>8923847</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>1</v>
+      <c r="H24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="str" cm="1">
+        <f t="array" ref="A27:A29">_xlfn._xlws.FILTER(A15:A24,COUNTIF(E15:E24,A15:A24))</f>
+        <v>Clash of Clans</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="str">
+        <v>Candy Crush Saga</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="str">
+        <v>Subway Surfers</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>